<commit_message>
Update Print Summary Data
</commit_message>
<xml_diff>
--- a/print_summary/wht-summary-2016-08-29.xlsx
+++ b/print_summary/wht-summary-2016-08-29.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="165">
   <si>
     <t>หนังสือรับรอง</t>
   </si>
@@ -512,6 +512,9 @@
   </si>
   <si>
     <t>66/2-4 หมู่3 ต. ทุ่งเบญจา อ.ท่าใหม่ จันทบุรี 22170</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -2514,12 +2517,18 @@
       <c r="A53" s="9"/>
       <c r="B53" s="10"/>
       <c r="C53" s="30"/>
-      <c r="D53" s="31"/>
+      <c r="D53" s="31" t="s">
+        <v>164</v>
+      </c>
       <c r="E53" s="6"/>
       <c r="F53" s="11"/>
       <c r="G53" s="12"/>
-      <c r="H53" s="13"/>
-      <c r="I53" s="14"/>
+      <c r="H53" s="13">
+        <v>2591327</v>
+      </c>
+      <c r="I53" s="14">
+        <v>82508.19</v>
+      </c>
       <c r="J53" s="5"/>
     </row>
     <row r="54" spans="1:13" customHeight="1" ht="21.75">

</xml_diff>